<commit_message>
large code cleanup and addition of some indicators
</commit_message>
<xml_diff>
--- a/resources/btc-bb.xlsx
+++ b/resources/btc-bb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E1BCFB-AE46-4D76-A0D1-3437307A55C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97926CF-EC9B-45AD-A14F-FE3242E50584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22920" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -370,7 +370,7 @@
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,132 +378,276 @@
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1515669120</v>
       </c>
       <c r="B1">
         <v>13319</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1515669180</v>
       </c>
       <c r="B2">
         <v>13319</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1515669240</v>
       </c>
       <c r="B3">
         <v>13346.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1515669300</v>
       </c>
       <c r="B4">
         <v>13346.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1515669360</v>
       </c>
       <c r="B5">
         <v>13346.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1515669420</v>
       </c>
       <c r="B6">
         <v>13273.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1515669480</v>
       </c>
       <c r="B7">
         <v>13274.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1515669540</v>
       </c>
       <c r="B8">
         <v>13230</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1515669600</v>
       </c>
       <c r="B9">
         <v>13311.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1515669660</v>
       </c>
       <c r="B10">
         <v>13274.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1515669720</v>
       </c>
       <c r="B11">
         <v>13294.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1515669780</v>
       </c>
       <c r="B12">
         <v>13348.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1515669840</v>
       </c>
       <c r="B13">
         <v>13348</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1515669900</v>
       </c>
       <c r="B14">
         <v>13321.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1515669960</v>
       </c>
       <c r="B15">
         <v>13311</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1515670020</v>
       </c>
       <c r="B16">
         <v>13322.1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,6 +657,15 @@
       <c r="B17">
         <v>13322.1</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -521,6 +674,15 @@
       <c r="B18">
         <v>13330</v>
       </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -529,6 +691,15 @@
       <c r="B19">
         <v>13292.1</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -4152,5 +4323,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="C20:C200 D20:D1048576 E20:E1048576" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>